<commit_message>
created scripts for Login and started with FT-Suppliers
</commit_message>
<xml_diff>
--- a/data/input.xlsx
+++ b/data/input.xlsx
@@ -5,15 +5,15 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\git\b72framework2\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\B77\WorkSpace\pos\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29AC215A-46D6-4393-811C-C6DBCB2D4797}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{850F6749-D56D-423B-884D-04453C9B054A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="ValidLogin" sheetId="2" r:id="rId1"/>
+    <sheet name="POS_Login" sheetId="2" r:id="rId1"/>
     <sheet name="InvalidLogin" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="10">
   <si>
     <t>admin</t>
   </si>
@@ -37,9 +37,6 @@
     <t>Password</t>
   </si>
   <si>
-    <t>manager</t>
-  </si>
-  <si>
     <t>damager</t>
   </si>
   <si>
@@ -47,6 +44,18 @@
   </si>
   <si>
     <t>xyz456</t>
+  </si>
+  <si>
+    <t>nopoint</t>
+  </si>
+  <si>
+    <t>bhanu</t>
+  </si>
+  <si>
+    <t>pointofsale</t>
+  </si>
+  <si>
+    <t>POINTOFSALE</t>
   </si>
 </sst>
 </file>
@@ -62,15 +71,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -78,12 +93,29 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -364,28 +396,70 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D44681BB-C97D-4DEB-B4B6-F5F64E22853C}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView zoomScale="220" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
-        <v>3</v>
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="2"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="2"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+      <c r="B8" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -397,8 +471,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C5B7C27-EE34-4AF6-8CFE-7FAEC6C4CFBF}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -413,10 +487,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
         <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -424,7 +498,7 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>